<commit_message>
added final rev2 protoboard for BQ76920
</commit_message>
<xml_diff>
--- a/Boards/BatteryManagementTest/BQ76920 Protoboard 2 BoM.xlsx
+++ b/Boards/BatteryManagementTest/BQ76920 Protoboard 2 BoM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>Reference Designator</t>
   </si>
@@ -54,30 +54,12 @@
     <t>296-39960-1-ND</t>
   </si>
   <si>
-    <t>C1, C2</t>
-  </si>
-  <si>
     <t>1uF Capacitor</t>
   </si>
   <si>
-    <t>C3</t>
-  </si>
-  <si>
     <t>.1uF Capacitor</t>
   </si>
   <si>
-    <t>CL05A104MP5NNNC</t>
-  </si>
-  <si>
-    <t>1276-1443-1-ND</t>
-  </si>
-  <si>
-    <t>R_SHUNT</t>
-  </si>
-  <si>
-    <t>Bourns Inc.</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -93,21 +75,128 @@
     <t>497-17143-1-ND</t>
   </si>
   <si>
-    <t>CRE2512-FZ-R005E-3CT-ND</t>
-  </si>
-  <si>
-    <t>5m Shunt</t>
-  </si>
-  <si>
-    <t>CRE2512-FZ-R005E-3</t>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Toshiba Semiconductor and Storage</t>
+  </si>
+  <si>
+    <t>CUS08F30,H3F</t>
+  </si>
+  <si>
+    <t>CUS08F30H3FCT-ND</t>
+  </si>
+  <si>
+    <t>10k Resistor</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>100 Resistor</t>
+  </si>
+  <si>
+    <t>A126330CT-ND</t>
+  </si>
+  <si>
+    <t>CRG0603J100R</t>
+  </si>
+  <si>
+    <t>TE Connectivity Passive Product</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>2.2uF Capacitor</t>
+  </si>
+  <si>
+    <t>490-10486-1-ND</t>
+  </si>
+  <si>
+    <t>GRM188R6YA225MA12D</t>
+  </si>
+  <si>
+    <t>Murata Electronics North America</t>
+  </si>
+  <si>
+    <t>399-17575-1-ND</t>
+  </si>
+  <si>
+    <t>C0603C104K9PAC7867</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C1, C3</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R5, R6</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>499k Resistor</t>
+  </si>
+  <si>
+    <t>Panasonic Electronic Components</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF4993V</t>
+  </si>
+  <si>
+    <t>P499KHCT-ND</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>We already have these for sure so no need to buy them</t>
+  </si>
+  <si>
+    <t>220mV Schottkey Diode</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>50m Shunt Resistor</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>PE2512FKE070R05L</t>
+  </si>
+  <si>
+    <t>YAG2156CT-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -142,7 +231,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -165,21 +254,219 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,117 +782,311 @@
     <col min="4" max="4" width="27.7109375" customWidth="1"/>
     <col min="5" max="5" width="16.140625" customWidth="1"/>
     <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="G1" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="G2" s="4">
+        <v>4</v>
+      </c>
+      <c r="H2" s="6">
+        <v>2.89</v>
+      </c>
+      <c r="I2">
+        <f>G2*H2</f>
+        <v>11.56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4">
+        <v>3</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0.99</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I9" si="0">G3*H3</f>
+        <v>2.9699999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="4">
+        <v>3</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0.36</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="4">
+        <v>3</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0.30000000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="4">
+        <v>3</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0.30000000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="4">
+        <v>3</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="4">
+        <v>6</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.21</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="22">
+        <v>3</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.26</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" s="24">
+        <f>SUM(I2:I9)</f>
+        <v>20.320000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="19"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>24</v>
-      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="2"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>